<commit_message>
20200310 오후05:59 book_main_category랑 book_sub_category추가
</commit_message>
<xml_diff>
--- a/20200310 db 칼럼+제약 조건.xlsx
+++ b/20200310 db 칼럼+제약 조건.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="209">
   <si>
     <t>Member</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -644,6 +644,214 @@
   </si>
   <si>
     <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book_main_category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 카테고리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>novel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self_development</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>health_diet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>computer_it</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>business_economy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서브 카테고리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book_sub_category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제약조건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소설</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기 계발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건강_다이어트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외국어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터_IT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경제_경영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소설전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판타지_무협</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로맨스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기계발 전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성공_삶의 자세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>취업_창업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설득_화술_협상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건강_다이어트 전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스마일_뷰티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동_스포츠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외국어 전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비스니스 영어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반영어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제2외국어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터_IT전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT비즈니스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT자격증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발_프로그래밍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT해외원서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경영_경제 전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경영 일반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경제 일반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마케팅_세일즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CEO_리더쉽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_category_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_category_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_category_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_category_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -682,7 +890,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1006,13 +1214,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1126,6 +1356,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1426,16 +1665,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:AE102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.75" customWidth="1"/>
     <col min="4" max="4" width="17.125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
@@ -1445,18 +1684,18 @@
     <col min="9" max="9" width="14.75" customWidth="1"/>
     <col min="10" max="10" width="14.375" customWidth="1"/>
     <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.875" customWidth="1"/>
-    <col min="13" max="13" width="28.625" customWidth="1"/>
-    <col min="14" max="14" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="31" width="14.375" customWidth="1"/>
+    <col min="32" max="32" width="28.625" customWidth="1"/>
+    <col min="33" max="33" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17.25" thickBot="1"/>
-    <row r="2" spans="1:19" ht="18" thickTop="1" thickBot="1">
+    <row r="1" spans="1:31" ht="17.25" thickBot="1"/>
+    <row r="2" spans="1:31" ht="18" thickTop="1" thickBot="1">
       <c r="B2" s="34" t="s">
         <v>8</v>
       </c>
@@ -1471,17 +1710,28 @@
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
-      <c r="L2" s="37"/>
-      <c r="N2" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="13"/>
-    </row>
-    <row r="3" spans="1:19" ht="17.25" thickTop="1">
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="37"/>
+    </row>
+    <row r="3" spans="1:31" ht="17.25" thickTop="1">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1511,27 +1761,28 @@
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="27"/>
-      <c r="N3" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="27"/>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1565,116 +1816,123 @@
       <c r="K4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="L4" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="28"/>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="27"/>
-      <c r="N5" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="7"/>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="27"/>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>165</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="27"/>
-      <c r="N6" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="7"/>
-    </row>
-    <row r="7" spans="1:19">
+        <v>203</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="28"/>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1683,68 +1941,82 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="27"/>
-      <c r="N7" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="27"/>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="27"/>
-      <c r="N8" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="S8" s="10"/>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="27"/>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>1</v>
@@ -1752,189 +2024,245 @@
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="27"/>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:19" ht="17.25" thickBot="1">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="27"/>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="27"/>
+    </row>
+    <row r="12" spans="1:31">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="27"/>
+    </row>
+    <row r="13" spans="1:31" ht="17.25" thickBot="1">
+      <c r="A13" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B13" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C13" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D13" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E13" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F13" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G13" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
-    </row>
-    <row r="12" spans="1:19" ht="17.25" thickTop="1"/>
-    <row r="13" spans="1:19" ht="17.25" thickBot="1"/>
-    <row r="14" spans="1:19" ht="17.25" thickBot="1">
-      <c r="B14" s="11" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="31"/>
+    </row>
+    <row r="14" spans="1:31" ht="17.25" thickTop="1"/>
+    <row r="16" spans="1:31">
+      <c r="B16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" t="s">
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-      <c r="L14" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="B15" s="6" t="s">
+      <c r="I16" s="12"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="2:31">
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="17.25" thickBot="1">
-      <c r="B16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11">
-      <c r="B17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1942,23 +2270,47 @@
         <v>44</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="J17" s="7" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
+        <v>99</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+    </row>
+    <row r="18" spans="2:31">
       <c r="B18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
@@ -1968,25 +2320,45 @@
         <v>44</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>12</v>
+        <v>101</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="1" t="s">
-        <v>43</v>
+      <c r="I18" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>44</v>
+        <v>156</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11">
+        <v>153</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+    </row>
+    <row r="19" spans="2:31">
       <c r="B19" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
@@ -1996,25 +2368,43 @@
         <v>44</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>13</v>
+        <v>102</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="I19" s="1"/>
       <c r="J19" s="7" t="s">
         <v>44</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11">
+        <v>154</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+    </row>
+    <row r="20" spans="2:31">
       <c r="B20" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
@@ -2024,10 +2414,10 @@
         <v>44</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
@@ -2037,25 +2427,45 @@
         <v>44</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+    </row>
+    <row r="21" spans="2:31">
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="7" t="s">
         <v>44</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
@@ -2065,17 +2475,45 @@
         <v>44</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+    </row>
+    <row r="22" spans="2:31">
+      <c r="B22" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="4"/>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="G22" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
@@ -2085,89 +2523,205 @@
         <v>44</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11">
+        <v>80</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+    </row>
+    <row r="23" spans="2:31">
+      <c r="B23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="G23" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+    </row>
+    <row r="24" spans="2:31">
+      <c r="B24" s="4"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+    </row>
+    <row r="25" spans="2:31">
+      <c r="G25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="11" t="s">
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+    </row>
+    <row r="26" spans="2:31">
+      <c r="B26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C26" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
+      <c r="F26" t="s">
         <v>72</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G26" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="16" t="s">
+      <c r="H26" s="9"/>
+      <c r="I26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J26" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="2:11">
-      <c r="B25" s="14" t="s">
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+    </row>
+    <row r="27" spans="2:31">
+      <c r="B27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="B26" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11">
-      <c r="B27" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
         <v>43</v>
       </c>
@@ -2175,22 +2729,16 @@
         <v>44</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="2:11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31">
       <c r="B28" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>43</v>
       </c>
@@ -2198,27 +2746,12 @@
         <v>44</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K28" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:31">
       <c r="B29" s="14" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
@@ -2228,139 +2761,201 @@
         <v>44</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="2:31">
+      <c r="B30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+    </row>
+    <row r="31" spans="2:31">
+      <c r="B31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G31" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J31" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" s="15" t="s">
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+    </row>
+    <row r="32" spans="2:31">
+      <c r="B32" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9" t="s">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="2:11">
-      <c r="G31" s="11" t="s">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="2:31">
+      <c r="G33" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="H33" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="11" t="s">
+      <c r="I33" s="12"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="2:31">
+      <c r="B34" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-      <c r="F32" t="s">
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+      <c r="F34" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="J34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="2:11">
-      <c r="B33" s="14" t="s">
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+    </row>
+    <row r="35" spans="2:31">
+      <c r="B35" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11">
-      <c r="B34" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="2:11">
-      <c r="B35" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
         <v>43</v>
       </c>
@@ -2368,83 +2963,138 @@
         <v>44</v>
       </c>
       <c r="F35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+    </row>
+    <row r="36" spans="2:31">
+      <c r="B36" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="2:31">
+      <c r="B37" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G37" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H37" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="2:11">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="G36" s="6" t="s">
+      <c r="I37" s="12"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="2:31">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="G38" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="G37" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="G38" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="H38" s="1"/>
       <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="22" t="s">
-        <v>68</v>
+      <c r="J38" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11">
+        <v>114</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
+      <c r="AC38" s="4"/>
+      <c r="AD38" s="4"/>
+      <c r="AE38" s="4"/>
+    </row>
+    <row r="39" spans="2:31">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
       <c r="G39" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H39" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="I39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2452,91 +3102,262 @@
         <v>44</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
+      <c r="AC39" s="4"/>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="4"/>
+    </row>
+    <row r="40" spans="2:31">
+      <c r="B40" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
       <c r="G40" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H40" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="I40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="J40" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="4"/>
+    </row>
+    <row r="41" spans="2:31">
+      <c r="B41" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="F41" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="4"/>
+    </row>
+    <row r="42" spans="2:31">
+      <c r="B42" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="2:11">
-      <c r="G41" s="8" t="s">
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="4"/>
+    </row>
+    <row r="43" spans="2:31">
+      <c r="B43" s="40"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="G43" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9" t="s">
+      <c r="H43" s="9"/>
+      <c r="I43" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J43" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="2:11">
-      <c r="G43" s="11" t="s">
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="4"/>
+      <c r="AE43" s="4"/>
+    </row>
+    <row r="44" spans="2:31">
+      <c r="B44" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
+    </row>
+    <row r="45" spans="2:31">
+      <c r="B45" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H45" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-    </row>
-    <row r="44" spans="2:11">
-      <c r="G44" s="14" t="s">
+      <c r="I45" s="12"/>
+      <c r="J45" s="13"/>
+    </row>
+    <row r="46" spans="2:31">
+      <c r="B46" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G46" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" ht="82.5">
-      <c r="G45" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J45" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11">
-      <c r="G46" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H46" s="1"/>
       <c r="I46" s="1" t="s">
         <v>43</v>
       </c>
@@ -2544,42 +3365,763 @@
         <v>44</v>
       </c>
       <c r="K46" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+    </row>
+    <row r="47" spans="2:31" ht="33">
+      <c r="G47" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="4"/>
+    </row>
+    <row r="48" spans="2:31">
+      <c r="G48" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="47" spans="2:11">
-      <c r="G47" s="14" t="s">
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4"/>
+      <c r="AE48" s="4"/>
+    </row>
+    <row r="49" spans="7:31">
+      <c r="G49" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1" t="s">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J47" s="7" t="s">
+      <c r="J49" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="48" spans="2:11">
-      <c r="G48" s="8" t="s">
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+    </row>
+    <row r="50" spans="7:31">
+      <c r="G50" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9" t="s">
+      <c r="H50" s="9"/>
+      <c r="I50" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="J48" s="10" t="s">
+      <c r="J50" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K50" s="4" t="s">
         <v>151</v>
+      </c>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="4"/>
+      <c r="AE50" s="4"/>
+    </row>
+    <row r="52" spans="7:31" ht="17.25" thickBot="1"/>
+    <row r="53" spans="7:31" ht="17.25" thickBot="1">
+      <c r="G53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H53" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="7:31">
+      <c r="G54" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="7:31" ht="17.25" thickBot="1">
+      <c r="G55" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="7:31">
+      <c r="G57" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="13"/>
+    </row>
+    <row r="58" spans="7:31">
+      <c r="G58" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="7:31">
+      <c r="G59" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="L59" s="7"/>
+    </row>
+    <row r="60" spans="7:31">
+      <c r="G60" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K60" s="1"/>
+      <c r="L60" s="7"/>
+    </row>
+    <row r="61" spans="7:31">
+      <c r="G61" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="L61" s="7"/>
+    </row>
+    <row r="62" spans="7:31">
+      <c r="G62" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="L62" s="7"/>
+    </row>
+    <row r="63" spans="7:31">
+      <c r="G63" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="K63" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="L63" s="10"/>
+    </row>
+    <row r="66" spans="6:13">
+      <c r="G66" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="13"/>
+    </row>
+    <row r="67" spans="6:13">
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="I67" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="6:13">
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="I68" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="6:13">
+      <c r="F69">
+        <v>3</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="I69" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="6:13">
+      <c r="F70">
+        <v>4</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J70" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="6:13">
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="6:13">
+      <c r="F72">
+        <v>6</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H72" s="9"/>
+      <c r="I72" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="6:13">
+      <c r="G74" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H74" s="12"/>
+      <c r="I74" s="13"/>
+    </row>
+    <row r="75" spans="6:13">
+      <c r="G75" s="39">
+        <v>100</v>
+      </c>
+      <c r="H75" s="5"/>
+      <c r="I75" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J75" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="6:13">
+      <c r="G76" s="6">
+        <v>101</v>
+      </c>
+      <c r="H76" s="1"/>
+      <c r="I76" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J76" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="6:13">
+      <c r="G77" s="6">
+        <v>102</v>
+      </c>
+      <c r="H77" s="1"/>
+      <c r="I77" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J77" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" spans="6:13">
+      <c r="G78" s="6">
+        <v>103</v>
+      </c>
+      <c r="H78" s="1"/>
+      <c r="I78" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="6:13">
+      <c r="G79" s="6">
+        <v>104</v>
+      </c>
+      <c r="H79" s="1"/>
+      <c r="I79" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J79" t="s">
+        <v>180</v>
+      </c>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+    </row>
+    <row r="80" spans="6:13">
+      <c r="G80" s="8">
+        <v>105</v>
+      </c>
+      <c r="H80" s="9"/>
+      <c r="I80" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J80" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="7:10">
+      <c r="G81" s="6">
+        <v>200</v>
+      </c>
+      <c r="H81" s="1"/>
+      <c r="I81" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="7:10">
+      <c r="G82" s="6">
+        <v>201</v>
+      </c>
+      <c r="H82" s="1"/>
+      <c r="I82" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J82" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="7:10">
+      <c r="G83" s="6">
+        <v>202</v>
+      </c>
+      <c r="H83" s="1"/>
+      <c r="I83" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J83" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="84" spans="7:10">
+      <c r="G84" s="6">
+        <v>203</v>
+      </c>
+      <c r="H84" s="1"/>
+      <c r="I84" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J84" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" spans="7:10">
+      <c r="G85" s="39">
+        <v>300</v>
+      </c>
+      <c r="H85" s="5"/>
+      <c r="I85" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J85" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" spans="7:10">
+      <c r="G86" s="6">
+        <v>301</v>
+      </c>
+      <c r="H86" s="1"/>
+      <c r="I86" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J86" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="87" spans="7:10">
+      <c r="G87" s="6">
+        <v>302</v>
+      </c>
+      <c r="H87" s="1"/>
+      <c r="I87" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J87" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="7:10">
+      <c r="G88" s="8">
+        <v>303</v>
+      </c>
+      <c r="H88" s="9"/>
+      <c r="I88" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J88" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="7:10">
+      <c r="G89" s="6">
+        <v>400</v>
+      </c>
+      <c r="H89" s="1"/>
+      <c r="I89" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J89" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="7:10">
+      <c r="G90" s="6">
+        <v>401</v>
+      </c>
+      <c r="H90" s="1"/>
+      <c r="I90" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J90" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="91" spans="7:10">
+      <c r="G91" s="6">
+        <v>402</v>
+      </c>
+      <c r="H91" s="1"/>
+      <c r="I91" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="7:10">
+      <c r="G92" s="6">
+        <v>403</v>
+      </c>
+      <c r="H92" s="1"/>
+      <c r="I92" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J92" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="7:10">
+      <c r="G93" s="39">
+        <v>500</v>
+      </c>
+      <c r="H93" s="5"/>
+      <c r="I93" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J93" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="94" spans="7:10">
+      <c r="G94" s="6">
+        <v>501</v>
+      </c>
+      <c r="H94" s="1"/>
+      <c r="I94" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J94" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="7:10">
+      <c r="G95" s="6">
+        <v>502</v>
+      </c>
+      <c r="H95" s="1"/>
+      <c r="I95" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J95" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="96" spans="7:10">
+      <c r="G96" s="6">
+        <v>503</v>
+      </c>
+      <c r="H96" s="1"/>
+      <c r="I96" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J96" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="97" spans="7:10">
+      <c r="G97" s="8">
+        <v>504</v>
+      </c>
+      <c r="H97" s="9"/>
+      <c r="I97" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J97" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="7:10">
+      <c r="G98" s="6">
+        <v>600</v>
+      </c>
+      <c r="H98" s="1"/>
+      <c r="I98" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J98" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="99" spans="7:10">
+      <c r="G99" s="6">
+        <v>601</v>
+      </c>
+      <c r="H99" s="1"/>
+      <c r="I99" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J99" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="7:10">
+      <c r="G100" s="6">
+        <v>602</v>
+      </c>
+      <c r="H100" s="1"/>
+      <c r="I100" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J100" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="7:10">
+      <c r="G101" s="6">
+        <v>603</v>
+      </c>
+      <c r="H101" s="1"/>
+      <c r="I101" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="7:10">
+      <c r="G102" s="8">
+        <v>604</v>
+      </c>
+      <c r="H102" s="9"/>
+      <c r="I102" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="J102" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="C2:AE2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>